<commit_message>
P4: Todo al completo
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -3,17 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mg+FFFy8Km7JuM4aUaNIZyzSuysZw=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
-  <si>
-    <t>EQUIPO:                                           (fecha)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+  <si>
+    <t>EQUIPO:                                           25/05/2021</t>
   </si>
   <si>
     <t>TEST A:</t>
@@ -25,7 +30,30 @@
     <t xml:space="preserve">DISEÑO DE INTERFACES DE USUARIO </t>
   </si>
   <si>
-    <t xml:space="preserve">Web: </t>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Web: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/corderop/DIU21/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Web: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/MiguelangelX72/DIU21/</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PRACTICA 4 - Cuestionario SUS </t>
@@ -40,33 +68,60 @@
     <t xml:space="preserve">USUARIO ID: </t>
   </si>
   <si>
-    <t>#USER1</t>
-  </si>
-  <si>
-    <t>#USER2</t>
-  </si>
-  <si>
-    <t>#USER3</t>
-  </si>
-  <si>
-    <t>#USER4</t>
-  </si>
-  <si>
     <t>SEXO</t>
   </si>
   <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
     <t>EDAD</t>
   </si>
   <si>
     <t>OCUPACION</t>
   </si>
   <si>
+    <t>Desempleado</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>Jubilada</t>
+  </si>
+  <si>
+    <t>Director de banco</t>
+  </si>
+  <si>
     <t>EXPERIENCIA TIC</t>
   </si>
   <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
     <t>PERFIL (describir)</t>
   </si>
   <si>
+    <t>Amigable, Fotógrafo, Asustado</t>
+  </si>
+  <si>
+    <t>Trabajadora, Bailar, Feliz</t>
+  </si>
+  <si>
+    <t>Familiar, Hablar idioma, Enfadada</t>
+  </si>
+  <si>
+    <t>Trabajador, estudiar, disgustado</t>
+  </si>
+  <si>
     <t>1: Completamente en desacuerdo</t>
   </si>
   <si>
@@ -77,17 +132,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>User1</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
@@ -96,49 +159,73 @@
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>User2</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>User3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>User3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
@@ -183,65 +270,97 @@
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">MARGINAL </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>D</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve"> (ENTRE 60-70)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t>ACEPTABLE TIPO</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> C </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t>(GOOD 70-80)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">ACEPTABLE TIPO </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">B </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t>(EXECELENT 70-80)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t xml:space="preserve">ACEPTABLE TIPO </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">A </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
       <t>(THE BEST 90-100)</t>
     </r>
   </si>
@@ -256,7 +375,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -264,18 +383,34 @@
     </font>
     <font/>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="12.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -303,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border/>
     <border>
       <left style="thick">
@@ -387,40 +522,6 @@
       </bottom>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF0000FF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF00FF00"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF00FF00"/>
-      </right>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
@@ -461,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -469,121 +570,116 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="12" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="14" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -607,6 +703,200 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+  <a:themeElements>
+    <a:clrScheme name="Sheets">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="0000FF"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Sheets">
+      <a:majorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -622,7 +912,9 @@
     <col customWidth="1" min="2" max="2" width="50.71"/>
     <col customWidth="1" min="3" max="3" width="27.86"/>
     <col customWidth="1" hidden="1" min="4" max="4" width="27.86"/>
-    <col customWidth="1" min="5" max="7" width="27.86"/>
+    <col customWidth="1" min="5" max="5" width="27.86"/>
+    <col customWidth="1" min="6" max="6" width="32.14"/>
+    <col customWidth="1" min="7" max="7" width="31.71"/>
     <col customWidth="1" min="8" max="8" width="22.0"/>
   </cols>
   <sheetData>
@@ -630,445 +922,565 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" ht="15.0" customHeight="1">
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10">
+        <v>352.0</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12">
+        <v>533.0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>221.0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>515.0</v>
+      </c>
+    </row>
+    <row r="5" ht="15.0" customHeight="1">
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="15.0" customHeight="1">
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42.0</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12">
+        <v>33.0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>66.0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="7" ht="15.0" customHeight="1">
+      <c r="B7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="15.0" customHeight="1">
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" ht="9.75" customHeight="1">
+      <c r="B10" s="9"/>
+      <c r="C10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="C11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="C12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="31">
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="32">
+        <f>C14-1</f>
+        <v>2</v>
+      </c>
+      <c r="E14" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="F14" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="G14" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1">
+      <c r="A15" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="32">
+        <f>5-C15</f>
+        <v>3</v>
+      </c>
+      <c r="E15" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="G15" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+    </row>
+    <row r="16" ht="25.5" customHeight="1">
+      <c r="A16" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="31">
+        <v>4.0</v>
+      </c>
+      <c r="D16" s="32">
+        <f>C16-1</f>
+        <v>3</v>
+      </c>
+      <c r="E16" s="33">
+        <v>5.0</v>
+      </c>
+      <c r="F16" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="G16" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" ht="25.5" customHeight="1">
+      <c r="A17" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="D17" s="32">
+        <f>5-C17</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="G17" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" ht="25.5" customHeight="1">
+      <c r="A18" s="29">
+        <v>5.0</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="31">
+        <v>4.0</v>
+      </c>
+      <c r="D18" s="32">
+        <f>C18-1</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="F18" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="G18" s="35">
+        <v>2.0</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" ht="25.5" customHeight="1">
+      <c r="A19" s="29">
+        <v>6.0</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="D19" s="32">
+        <f>5-C19</f>
+        <v>3</v>
+      </c>
+      <c r="E19" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="F19" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="G19" s="35">
+        <v>3.0</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" ht="25.5" customHeight="1">
+      <c r="A20" s="29">
+        <v>7.0</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="31">
+        <v>5.0</v>
+      </c>
+      <c r="D20" s="32">
+        <f>C20-1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" ht="15.0" customHeight="1">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="15.0" customHeight="1">
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" ht="15.0" customHeight="1">
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" ht="15.0" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" ht="15.0" customHeight="1">
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" ht="9.75" customHeight="1">
-      <c r="B10" s="7"/>
-      <c r="C10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="C12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="25">
+      <c r="E20" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="F20" s="34">
+        <v>4.0</v>
+      </c>
+      <c r="G20" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" ht="25.5" customHeight="1">
+      <c r="A21" s="29">
+        <v>8.0</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="31">
         <v>1.0</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28">
-        <f>C14-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" ht="25.5" customHeight="1">
-      <c r="A15" s="25">
+      <c r="D21" s="32">
+        <f>5-C21</f>
+        <v>4</v>
+      </c>
+      <c r="E21" s="33">
         <v>2.0</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28">
-        <f>5-C15</f>
-        <v>5</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" s="25">
+      <c r="F21" s="34">
+        <v>4.0</v>
+      </c>
+      <c r="G21" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="22" ht="25.5" customHeight="1">
+      <c r="A22" s="29">
+        <v>9.0</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="31">
         <v>3.0</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28">
-        <f>C16-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-    </row>
-    <row r="17" ht="25.5" customHeight="1">
-      <c r="A17" s="25">
+      <c r="D22" s="32">
+        <f>C22-1</f>
+        <v>2</v>
+      </c>
+      <c r="E22" s="33">
         <v>4.0</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28">
-        <f>5-C17</f>
-        <v>5</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="18" ht="25.5" customHeight="1">
-      <c r="A18" s="25">
-        <v>5.0</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28">
-        <f>C18-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" ht="25.5" customHeight="1">
-      <c r="A19" s="25">
-        <v>6.0</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28">
-        <f>5-C19</f>
-        <v>5</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" s="25">
-        <v>7.0</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28">
-        <f>C20-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-    </row>
-    <row r="21" ht="25.5" customHeight="1">
-      <c r="A21" s="25">
-        <v>8.0</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28">
-        <f>5-C21</f>
-        <v>5</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-    </row>
-    <row r="22" ht="25.5" customHeight="1">
-      <c r="A22" s="25">
-        <v>9.0</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28">
-        <f>C22-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
+      <c r="F22" s="34">
+        <v>4.0</v>
+      </c>
+      <c r="G22" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" ht="25.5" customHeight="1">
-      <c r="A23" s="25">
+      <c r="A23" s="29">
         <v>10.0</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28">
+      <c r="B23" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="D23" s="32">
         <f>5-C23</f>
-        <v>5</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+        <v>3</v>
+      </c>
+      <c r="E23" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="F23" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="G23" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" ht="25.5" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="36">
         <f> ((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
-        <v>50</v>
-      </c>
-      <c r="D24" s="36">
+        <v>75</v>
+      </c>
+      <c r="D24" s="37">
         <f>(SUM(D14:D23))*2.5</f>
-        <v>50</v>
-      </c>
-      <c r="E24" s="37">
+        <v>75</v>
+      </c>
+      <c r="E24" s="38">
         <f t="shared" ref="E24:G24" si="1"> ((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
-        <v>50</v>
-      </c>
-      <c r="F24" s="38">
+        <v>80</v>
+      </c>
+      <c r="F24" s="39">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="40">
         <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" ht="25.5" customHeight="1">
+      <c r="B25" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="B26" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="B27" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="B28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-    </row>
-    <row r="25" ht="25.5" customHeight="1">
-      <c r="B25" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="41"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="42" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="42" t="s">
-        <v>41</v>
+      <c r="B29" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="42" t="s">
-        <v>42</v>
+      <c r="B30" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="1" t="s">
-        <v>43</v>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="43" t="s">
-        <v>44</v>
+      <c r="B34" s="42" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2037,13 +2449,6 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="C24 E24:G24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -2057,11 +2462,13 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B34"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="F2"/>
+    <hyperlink r:id="rId3" ref="B34"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToWidth="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>